<commit_message>
fix(redux slice): optimize redux slices
</commit_message>
<xml_diff>
--- a/public/self_perf_assessment.xlsx
+++ b/public/self_perf_assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\office\infobell\project1\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECFEC5F-9E47-459F-BD9E-925B52F4991C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78BB59D-6AF0-4743-BB76-DD30607274F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{EB4EC050-5F71-4C3A-A995-FEDFEE6643F0}"/>
+    <workbookView xWindow="2920" yWindow="2920" windowWidth="19200" windowHeight="11170" xr2:uid="{EB4EC050-5F71-4C3A-A995-FEDFEE6643F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>instance type</t>
   </si>
   <si>
     <t>performance score</t>
-  </si>
-  <si>
-    <t>m5a.12xLarge</t>
   </si>
 </sst>
 </file>
@@ -415,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38A2AC1-B8C5-40E4-8CB2-A0252B18C58F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -435,14 +432,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>145230</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>